<commit_message>
updated validation excel sheet
</commit_message>
<xml_diff>
--- a/validation/validation_results.xlsx
+++ b/validation/validation_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Skin Permeation\Skin-Permeation\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1854225-ED60-4119-ADD0-425770397F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D1493B-B907-4BB6-95CE-B8048A44E8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$16</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Compound name</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>diff_lightgbm</t>
+  </si>
+  <si>
+    <t>diff_catboost</t>
+  </si>
+  <si>
+    <t>diff_randomforest</t>
   </si>
   <si>
     <t>Cytarabine</t>
@@ -511,25 +520,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,208 +572,271 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>-4.3296974989999999</v>
+        <v>-5.2996974989999996</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F2">
-        <v>-2.7978325935908961</v>
+        <v>-3.680272961593789</v>
       </c>
       <c r="G2">
-        <v>-2.563592053913609</v>
+        <v>-3.273539318661022</v>
       </c>
       <c r="H2">
-        <v>-2.5182803945129031</v>
+        <v>-3.9354202964709311</v>
       </c>
       <c r="I2">
-        <v>-2.6265683473391359</v>
+        <v>-3.629744192241914</v>
       </c>
       <c r="J2">
-        <v>1.703129151660864</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.6699533067580861</v>
+      </c>
+      <c r="K2">
+        <v>1.364277202529069</v>
+      </c>
+      <c r="L2">
+        <v>2.0261581803389772</v>
+      </c>
+      <c r="M2">
+        <v>1.6194245374062111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>-5.2996974989999996</v>
+        <v>-3.332697499</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>305</v>
       </c>
       <c r="F3">
-        <v>-3.680272961593789</v>
+        <v>-3.5545331382798482</v>
       </c>
       <c r="G3">
-        <v>-3.273539318661022</v>
+        <v>-3.1833575876950988</v>
       </c>
       <c r="H3">
-        <v>-3.9354202964709311</v>
+        <v>-3.944206091934551</v>
       </c>
       <c r="I3">
-        <v>-3.629744192241914</v>
+        <v>-3.5606989393031658</v>
       </c>
       <c r="J3">
-        <v>1.6699533067580861</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.2280014403031658</v>
+      </c>
+      <c r="K3">
+        <v>0.61150859293455051</v>
+      </c>
+      <c r="L3">
+        <v>0.14933991130490121</v>
+      </c>
+      <c r="M3">
+        <v>0.2218356392798482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>-4.143697499</v>
+        <v>-2.1806974989999999</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>305</v>
+      </c>
+      <c r="F4">
+        <v>-3.020732738095238</v>
+      </c>
+      <c r="G4">
+        <v>-2.9674568936804628</v>
+      </c>
+      <c r="H4">
+        <v>-3.231940255559159</v>
+      </c>
+      <c r="I4">
+        <v>-3.0733766291116198</v>
+      </c>
+      <c r="J4">
+        <v>0.89267913011161992</v>
+      </c>
+      <c r="K4">
+        <v>1.0512427565591591</v>
+      </c>
+      <c r="L4">
+        <v>0.78675939468046341</v>
+      </c>
+      <c r="M4">
+        <v>0.8400352390952377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="E4">
-        <v>310</v>
-      </c>
-      <c r="F4">
-        <v>-2.7978325935908961</v>
-      </c>
-      <c r="G4">
-        <v>-2.563592053913609</v>
-      </c>
-      <c r="H4">
-        <v>-2.5182803945129031</v>
-      </c>
-      <c r="I4">
-        <v>-2.6265683473391359</v>
-      </c>
-      <c r="J4">
-        <v>1.517129151660864</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
       <c r="C5">
-        <v>-4.1746974989999996</v>
+        <v>-1.774697499</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>310</v>
       </c>
       <c r="F5">
-        <v>-2.8197650935908962</v>
+        <v>-2.937572831686134</v>
       </c>
       <c r="G5">
-        <v>-2.562996992615822</v>
+        <v>-2.6632253730772528</v>
       </c>
       <c r="H5">
-        <v>-2.591462968254274</v>
+        <v>-2.8010343956415471</v>
       </c>
       <c r="I5">
-        <v>-2.6580750181536641</v>
+        <v>-2.8006108668016449</v>
       </c>
       <c r="J5">
-        <v>1.516622480846336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.025913367801645</v>
+      </c>
+      <c r="K5">
+        <v>1.0263368966415469</v>
+      </c>
+      <c r="L5">
+        <v>0.88852787407725331</v>
+      </c>
+      <c r="M5">
+        <v>1.162875332686135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>-4.0376974990000001</v>
+        <v>-2.9206974990000001</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>310</v>
       </c>
       <c r="F6">
-        <v>-2.8197650935908962</v>
+        <v>-2.8088450935908962</v>
       </c>
       <c r="G6">
-        <v>-2.562996992615822</v>
+        <v>-2.5721227768554091</v>
       </c>
       <c r="H6">
         <v>-2.591462968254274</v>
       </c>
       <c r="I6">
-        <v>-2.6580750181536641</v>
+        <v>-2.6574769462335261</v>
       </c>
       <c r="J6">
-        <v>1.379622480846336</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.26322055276647388</v>
+      </c>
+      <c r="K6">
+        <v>0.32923453074572612</v>
+      </c>
+      <c r="L6">
+        <v>0.3485747221445914</v>
+      </c>
+      <c r="M6">
+        <v>0.11185240540910429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>-1.774697499</v>
+        <v>-3.3786974989999998</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>310</v>
       </c>
       <c r="F7">
-        <v>-2.937572831686134</v>
+        <v>-2.8088450935908962</v>
       </c>
       <c r="G7">
-        <v>-2.6632253730772528</v>
+        <v>-2.5721227768554091</v>
       </c>
       <c r="H7">
-        <v>-2.8010343956415471</v>
+        <v>-2.591462968254274</v>
       </c>
       <c r="I7">
-        <v>-2.8006108668016449</v>
+        <v>-2.6574769462335261</v>
       </c>
       <c r="J7">
-        <v>1.025913367801645</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.72122055276647368</v>
+      </c>
+      <c r="K7">
+        <v>0.7872345307457258</v>
+      </c>
+      <c r="L7">
+        <v>0.80657472214459114</v>
+      </c>
+      <c r="M7">
+        <v>0.56985240540910409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8">
-        <v>-3.6616974990000002</v>
+        <v>-1.9466974990000001</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -770,283 +845,360 @@
         <v>310</v>
       </c>
       <c r="F8">
-        <v>-2.8838149919648788</v>
+        <v>-2.9364371174004189</v>
       </c>
       <c r="G8">
-        <v>-2.6026615563081781</v>
+        <v>-2.6253055161400169</v>
       </c>
       <c r="H8">
-        <v>-2.8010343956415471</v>
+        <v>-2.7160593084182869</v>
       </c>
       <c r="I8">
-        <v>-2.7625036479715348</v>
+        <v>-2.7592673139862409</v>
       </c>
       <c r="J8">
-        <v>0.89919385102846539</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.81256981498624081</v>
+      </c>
+      <c r="K8">
+        <v>0.76936180941828725</v>
+      </c>
+      <c r="L8">
+        <v>0.67860801714001684</v>
+      </c>
+      <c r="M8">
+        <v>0.9897396184004188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>-2.1806974989999999</v>
+        <v>-3.3886974990000001</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E9">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F9">
-        <v>-3.020732738095238</v>
+        <v>-2.835328426924228</v>
       </c>
       <c r="G9">
-        <v>-2.9674568936804628</v>
+        <v>-2.5032734570458359</v>
       </c>
       <c r="H9">
-        <v>-3.231940255559159</v>
+        <v>-2.591462968254274</v>
       </c>
       <c r="I9">
-        <v>-3.0733766291116198</v>
+        <v>-2.643354950741446</v>
       </c>
       <c r="J9">
-        <v>0.89267913011161992</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.74534254825855406</v>
+      </c>
+      <c r="K9">
+        <v>0.79723453074572603</v>
+      </c>
+      <c r="L9">
+        <v>0.88542404195416413</v>
+      </c>
+      <c r="M9">
+        <v>0.55336907207577157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10">
+        <v>-2.9916974989999998</v>
+      </c>
+      <c r="D10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10">
-        <v>-1.9466974990000001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
       </c>
       <c r="E10">
         <v>310</v>
       </c>
       <c r="F10">
-        <v>-2.9364371174004189</v>
+        <v>-2.835328426924228</v>
       </c>
       <c r="G10">
-        <v>-2.6253055161400169</v>
+        <v>-2.5032734570458359</v>
       </c>
       <c r="H10">
-        <v>-2.7160593084182869</v>
+        <v>-2.591462968254274</v>
       </c>
       <c r="I10">
-        <v>-2.7592673139862409</v>
+        <v>-2.643354950741446</v>
       </c>
       <c r="J10">
-        <v>0.81256981498624081</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.34834254825855382</v>
+      </c>
+      <c r="K10">
+        <v>0.40023453074572579</v>
+      </c>
+      <c r="L10">
+        <v>0.48842404195416389</v>
+      </c>
+      <c r="M10">
+        <v>0.1563690720757713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C11">
-        <v>-3.3886974990000001</v>
+        <v>-2.594697499</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>310</v>
       </c>
       <c r="F11">
-        <v>-2.835328426924228</v>
+        <v>-2.937572831686134</v>
       </c>
       <c r="G11">
-        <v>-2.5032734570458359</v>
+        <v>-2.661001120813594</v>
       </c>
       <c r="H11">
-        <v>-2.591462968254274</v>
+        <v>-2.7871882653242359</v>
       </c>
       <c r="I11">
-        <v>-2.643354950741446</v>
+        <v>-2.795254072607988</v>
       </c>
       <c r="J11">
-        <v>0.74534254825855406</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.2005565736079884</v>
+      </c>
+      <c r="K11">
+        <v>0.1924907663242359</v>
+      </c>
+      <c r="L11">
+        <v>6.6303621813594393E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.34287533268613452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C12">
-        <v>-3.3786974989999998</v>
+        <v>-4.1746974989999996</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <v>310</v>
       </c>
       <c r="F12">
-        <v>-2.8088450935908962</v>
+        <v>-2.8197650935908962</v>
       </c>
       <c r="G12">
-        <v>-2.5721227768554091</v>
+        <v>-2.562996992615822</v>
       </c>
       <c r="H12">
         <v>-2.591462968254274</v>
       </c>
       <c r="I12">
-        <v>-2.6574769462335261</v>
+        <v>-2.6580750181536641</v>
       </c>
       <c r="J12">
-        <v>0.72122055276647368</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.516622480846336</v>
+      </c>
+      <c r="K12">
+        <v>1.5832345307457261</v>
+      </c>
+      <c r="L12">
+        <v>1.6117005063841769</v>
+      </c>
+      <c r="M12">
+        <v>1.354932405409103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C13">
-        <v>-2.9916974989999998</v>
+        <v>-4.0376974990000001</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E13">
         <v>310</v>
       </c>
       <c r="F13">
-        <v>-2.835328426924228</v>
+        <v>-2.8197650935908962</v>
       </c>
       <c r="G13">
-        <v>-2.5032734570458359</v>
+        <v>-2.562996992615822</v>
       </c>
       <c r="H13">
         <v>-2.591462968254274</v>
       </c>
       <c r="I13">
-        <v>-2.643354950741446</v>
+        <v>-2.6580750181536641</v>
       </c>
       <c r="J13">
-        <v>0.34834254825855382</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.379622480846336</v>
+      </c>
+      <c r="K13">
+        <v>1.4462345307457261</v>
+      </c>
+      <c r="L13">
+        <v>1.474700506384178</v>
+      </c>
+      <c r="M13">
+        <v>1.2179324054091041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>-2.9206974990000001</v>
+        <v>-3.6616974990000002</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>310</v>
       </c>
       <c r="F14">
-        <v>-2.8088450935908962</v>
+        <v>-2.8838149919648788</v>
       </c>
       <c r="G14">
-        <v>-2.5721227768554091</v>
+        <v>-2.6026615563081781</v>
       </c>
       <c r="H14">
-        <v>-2.591462968254274</v>
+        <v>-2.8010343956415471</v>
       </c>
       <c r="I14">
-        <v>-2.6574769462335261</v>
+        <v>-2.7625036479715348</v>
       </c>
       <c r="J14">
-        <v>0.26322055276647388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.89919385102846539</v>
+      </c>
+      <c r="K14">
+        <v>0.86066310335845309</v>
+      </c>
+      <c r="L14">
+        <v>1.059035942691823</v>
+      </c>
+      <c r="M14">
+        <v>0.77788250703512096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C15">
-        <v>-3.332697499</v>
+        <v>-4.3296974989999999</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E15">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="F15">
-        <v>-3.5545331382798482</v>
+        <v>-2.7978325935908961</v>
       </c>
       <c r="G15">
-        <v>-3.1833575876950988</v>
+        <v>-2.563592053913609</v>
       </c>
       <c r="H15">
-        <v>-3.944206091934551</v>
+        <v>-2.5182803945129031</v>
       </c>
       <c r="I15">
-        <v>-3.5606989393031658</v>
+        <v>-2.6265683473391359</v>
       </c>
       <c r="J15">
-        <v>0.2280014403031658</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.703129151660864</v>
+      </c>
+      <c r="K15">
+        <v>1.811417104487097</v>
+      </c>
+      <c r="L15">
+        <v>1.76610544508639</v>
+      </c>
+      <c r="M15">
+        <v>1.531864905409104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C16">
-        <v>-2.594697499</v>
+        <v>-4.143697499</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>310</v>
       </c>
       <c r="F16">
-        <v>-2.937572831686134</v>
+        <v>-2.7978325935908961</v>
       </c>
       <c r="G16">
-        <v>-2.661001120813594</v>
+        <v>-2.563592053913609</v>
       </c>
       <c r="H16">
-        <v>-2.7871882653242359</v>
+        <v>-2.5182803945129031</v>
       </c>
       <c r="I16">
-        <v>-2.795254072607988</v>
+        <v>-2.6265683473391359</v>
       </c>
       <c r="J16">
-        <v>0.2005565736079884</v>
+        <v>1.517129151660864</v>
+      </c>
+      <c r="K16">
+        <v>1.6254171044870971</v>
+      </c>
+      <c r="L16">
+        <v>1.5801054450863909</v>
+      </c>
+      <c r="M16">
+        <v>1.3458649054091041</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J16" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
-      <sortCondition descending="1" ref="J1:J16"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M16" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>